<commit_message>
Added first draft of testresults
</commit_message>
<xml_diff>
--- a/01_Dokumentation/08_Testresultate/Vortex_Tunnel_Test_29_Nov_2017.xlsx
+++ b/01_Dokumentation/08_Testresultate/Vortex_Tunnel_Test_29_Nov_2017.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tagroebe\Documents\Term_5\PAWI\pawi-vortex-tunnel-new\01_Dokumentation\08_Testresultate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DummyUser\Documents\Vortex\pawi-vortext-tunnel\01_Dokumentation\08_Testresultate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9410" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Standard" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="05 Wenige intensive Lichter" sheetId="7" r:id="rId6"/>
     <sheet name="06 Viele schwache Lichter" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="26">
   <si>
     <t>Mein Gleichgewichtssinn im Vortex Tunnel war beeinträchtigt</t>
   </si>
@@ -106,11 +106,14 @@
   <si>
     <t>Person 13</t>
   </si>
+  <si>
+    <t>Standard-Abweichung</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,16 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="16" max="16" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -514,8 +520,11 @@
       <c r="O1" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +571,12 @@
         <f>SUM(B2:K2)/10</f>
         <v>6.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P2">
+        <f>STDEVA(B2:N2)</f>
+        <v>2.5343790014670109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -610,8 +623,12 @@
         <f t="shared" ref="O3:O9" si="0">SUM(B3:K3)/10</f>
         <v>5.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="1">STDEVA(B3:N3)</f>
+        <v>2.7198227694899346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -658,8 +675,12 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>0.7679476477883046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -706,8 +727,12 @@
         <f t="shared" si="0"/>
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>2.063106942552968</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -739,8 +764,12 @@
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>0.91612538131290433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -787,8 +816,12 @@
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>1.3821202589704016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -835,8 +868,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>1.214231845389905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -882,6 +919,10 @@
       <c r="O9">
         <f t="shared" si="0"/>
         <v>2.7</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>2.3588350014578308</v>
       </c>
     </row>
   </sheetData>
@@ -892,18 +933,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -926,8 +967,14 @@
       <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,8 +1003,12 @@
         <f>SUM(B2:H2)/7</f>
         <v>4.2857142857142856</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <f>STDEVA(B2:H2)</f>
+        <v>1.4960264830861905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -986,8 +1037,12 @@
         <f t="shared" ref="I3:I8" si="0">SUM(B3:H3)/7</f>
         <v>4.4285714285714288</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="1">STDEVA(B3:H3)</f>
+        <v>3.1547394428670259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1016,8 +1071,12 @@
         <f t="shared" si="0"/>
         <v>2.2857142857142856</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.7043362064926935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1046,8 +1105,12 @@
         <f t="shared" si="0"/>
         <v>6.2857142857142856</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>2.4299715851758243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1067,8 +1130,12 @@
         <f t="shared" si="0"/>
         <v>1.1428571428571428</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>1.1547005383792515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1097,8 +1164,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>3.1622776601683795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,6 +1197,10 @@
       <c r="I8">
         <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
       </c>
     </row>
   </sheetData>
@@ -1135,18 +1210,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -1166,8 +1241,14 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1193,8 +1274,12 @@
         <f>SUM(B2:G2)/6</f>
         <v>6.333333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <f>STDEVA(B2:G2)</f>
+        <v>1.9663841605003505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1220,8 +1305,12 @@
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)/6</f>
         <v>5.166666666666667</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">STDEVA(B3:G3)</f>
+        <v>2.1369760566432814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1247,8 +1336,12 @@
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1.0327955589886444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1274,8 +1367,12 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.8708286933869707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1295,8 +1392,12 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1322,8 +1423,12 @@
         <f t="shared" si="0"/>
         <v>2.8333333333333335</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.8348478592697182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1348,6 +1453,10 @@
       <c r="H8">
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.40824829046386318</v>
       </c>
     </row>
   </sheetData>
@@ -1357,18 +1466,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -1391,8 +1500,14 @@
       <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1421,8 +1536,12 @@
         <f>SUM(B2:H2)/7</f>
         <v>5.4285714285714288</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <f>STDEVA(C2:H2)</f>
+        <v>2.3380903889000249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1451,8 +1570,12 @@
         <f t="shared" ref="I3:I8" si="0">SUM(B3:H3)/7</f>
         <v>4.4285714285714288</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="1">STDEVA(C3:H3)</f>
+        <v>3.0767948691238201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1481,8 +1604,12 @@
         <f t="shared" si="0"/>
         <v>2.7142857142857144</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.5055453054181622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1511,8 +1638,12 @@
         <f t="shared" si="0"/>
         <v>4.7142857142857144</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>1.366260102127947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1532,8 +1663,12 @@
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0.57735026918962573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1562,8 +1697,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>3.6560452221856705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1591,6 +1730,10 @@
       <c r="I8">
         <f t="shared" si="0"/>
         <v>1.8571428571428572</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.602081978759722</v>
       </c>
     </row>
   </sheetData>
@@ -1600,18 +1743,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -1631,8 +1774,14 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,8 +1807,12 @@
         <f>SUM(B2:G2)/6</f>
         <v>4.333333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <f>STDEVA(B2:G2)</f>
+        <v>2.2509257354845507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1685,8 +1838,12 @@
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)/6</f>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">STDEVA(B3:G3)</f>
+        <v>2.5099800796022267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1712,8 +1869,12 @@
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1.6329931618554521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1739,8 +1900,12 @@
         <f t="shared" si="0"/>
         <v>5.833333333333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>2.0412414523193156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1760,8 +1925,12 @@
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1787,8 +1956,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1813,6 +1986,10 @@
       <c r="H8">
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.40824829046386318</v>
       </c>
     </row>
   </sheetData>
@@ -1822,18 +1999,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -1856,8 +2033,14 @@
       <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1886,8 +2069,12 @@
         <f>SUM(B2:H2)/7</f>
         <v>4.4285714285714288</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <f>STDEVA(C2:H2)</f>
+        <v>2.0736441353327719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1916,8 +2103,12 @@
         <f t="shared" ref="I3:I8" si="0">SUM(B3:H3)/7</f>
         <v>3.8571428571428572</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="1">STDEVA(C3:H3)</f>
+        <v>2.2286019533929036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1946,8 +2137,12 @@
         <f t="shared" si="0"/>
         <v>3.1428571428571428</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.0954451150103321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1976,8 +2171,12 @@
         <f t="shared" si="0"/>
         <v>4.8571428571428568</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>2.1908902300206643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1997,8 +2196,12 @@
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0.57735026918962573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2027,8 +2230,12 @@
         <f t="shared" si="0"/>
         <v>5.2857142857142856</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>3.0767948691238205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2056,6 +2263,10 @@
       <c r="I8">
         <f t="shared" si="0"/>
         <v>2.1428571428571428</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.602081978759722</v>
       </c>
     </row>
   </sheetData>
@@ -2065,18 +2276,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -2096,8 +2307,14 @@
       <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2123,8 +2340,12 @@
         <f>SUM(B2:G2)/6</f>
         <v>5.666666666666667</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <f>STDEVA(B2:G2)</f>
+        <v>2.8751811537130436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2150,8 +2371,12 @@
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)/6</f>
         <v>5.333333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">STDEVA(B3:G3)</f>
+        <v>3.0110906108363245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2177,8 +2402,12 @@
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.40824829046386318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2204,8 +2433,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.8973665961010275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2225,8 +2458,12 @@
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2252,8 +2489,12 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.8708286933869707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2278,6 +2519,10 @@
       <c r="H8">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.2110601416389966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>